<commit_message>
running tests for dissertation
</commit_message>
<xml_diff>
--- a/profile data/profile data 2.0.0.xlsx
+++ b/profile data/profile data 2.0.0.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29520" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="12700" yWindow="740" windowWidth="29520" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hypothesis Test Analysis" sheetId="2" r:id="rId1"/>
@@ -109,9 +109,6 @@
     <t>H1:  Agent answer rate &gt; 0.25</t>
   </si>
   <si>
-    <t>Hypothesis Test Analysis: v. 1.5.0</t>
-  </si>
-  <si>
     <t>PROFILE</t>
   </si>
   <si>
@@ -164,6 +161,9 @@
   </si>
   <si>
     <t>all of above/definition/not</t>
+  </si>
+  <si>
+    <t>Hypothesis Test Analysis: v. 2.0.0</t>
   </si>
 </sst>
 </file>
@@ -820,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47:P47"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -832,7 +832,7 @@
   <sheetData>
     <row r="2" spans="2:19" ht="17">
       <c r="B2" s="4" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="2:19">
@@ -855,7 +855,7 @@
     </row>
     <row r="10" spans="2:19">
       <c r="S10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="2:19">
@@ -903,7 +903,7 @@
         <v>13</v>
       </c>
       <c r="S11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="2:19">
@@ -999,7 +999,7 @@
         <v>0.58699999999999997</v>
       </c>
       <c r="S13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="2:19">
@@ -1048,7 +1048,7 @@
         <v>0.77200000000000002</v>
       </c>
       <c r="S14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="2:19">
@@ -1134,7 +1134,7 @@
     </row>
     <row r="31" spans="2:19">
       <c r="S31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="2:19">
@@ -1182,7 +1182,7 @@
         <v>13</v>
       </c>
       <c r="S32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="2:19">
@@ -1278,7 +1278,7 @@
         <v>0.316</v>
       </c>
       <c r="S34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="2:19">
@@ -1327,7 +1327,7 @@
         <v>0.44800000000000001</v>
       </c>
       <c r="S35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="2:19">
@@ -1376,7 +1376,7 @@
         <v>0.35</v>
       </c>
       <c r="S36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="2:19">
@@ -1425,7 +1425,7 @@
         <v>0.188</v>
       </c>
       <c r="S37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="2:19">
@@ -1474,7 +1474,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="S38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="2:19">
@@ -1523,7 +1523,7 @@
         <v>0.40699999999999997</v>
       </c>
       <c r="S39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="2:19">
@@ -1572,7 +1572,7 @@
         <v>0.56299999999999994</v>
       </c>
       <c r="S40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="2:19">
@@ -1614,7 +1614,7 @@
         <v>0.36399999999999999</v>
       </c>
       <c r="S41" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="2:19">
@@ -1659,11 +1659,11 @@
         <v>0</v>
       </c>
       <c r="Q42">
-        <f>MAX(H42:P42)</f>
+        <f t="shared" ref="Q42:Q47" si="1">MAX(H42:P42)</f>
         <v>0.5</v>
       </c>
       <c r="S42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="2:19">
@@ -1701,11 +1701,11 @@
         <v>0.21299999999999999</v>
       </c>
       <c r="Q43">
-        <f>MAX(H43:P43)</f>
+        <f t="shared" si="1"/>
         <v>0.84299999999999997</v>
       </c>
       <c r="S43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="2:19">
@@ -1743,11 +1743,11 @@
         <v>0.23300000000000001</v>
       </c>
       <c r="Q44">
-        <f>MAX(H44:P44)</f>
+        <f t="shared" si="1"/>
         <v>0.85</v>
       </c>
       <c r="S44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="2:19">
@@ -1785,11 +1785,11 @@
         <v>0</v>
       </c>
       <c r="Q45">
-        <f>MAX(H45:P45)</f>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="S45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="2:19">
@@ -1827,11 +1827,11 @@
         <v>0</v>
       </c>
       <c r="Q46">
-        <f>MAX(H46:P46)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="2:19">
@@ -1869,11 +1869,11 @@
         <v>0</v>
       </c>
       <c r="Q47">
-        <f>MAX(H47:P47)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="S47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="7:17">

</xml_diff>